<commit_message>
updated and added at1 charts
</commit_message>
<xml_diff>
--- a/charting/data/Subordinate.xlsx
+++ b/charting/data/Subordinate.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbacher\Documents\Development\charting-lib\charting\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2049F90C-E665-414C-A7BA-5EC806FADA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDB94D4-0764-4B9F-838A-75AB347BD70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7F616339-BDE5-4F3E-AE3A-6EA6B9A512DF}"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="28830" windowHeight="15450" activeTab="1" xr2:uid="{7F616339-BDE5-4F3E-AE3A-6EA6B9A512DF}"/>
   </bookViews>
   <sheets>
     <sheet name="AT1" sheetId="1" r:id="rId1"/>
+    <sheet name="NON-FIN" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -35,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="163">
   <si>
     <t>YX500463 Corp</t>
   </si>
@@ -378,14 +401,162 @@
   </si>
   <si>
     <t>flt_spread().value</t>
+  </si>
+  <si>
+    <t>reset_index().value</t>
+  </si>
+  <si>
+    <t>EUAMDB05 Index</t>
+  </si>
+  <si>
+    <t>EUSA5 Index</t>
+  </si>
+  <si>
+    <t>EUR003M Index</t>
+  </si>
+  <si>
+    <t>SWAP_TO_CALL</t>
+  </si>
+  <si>
+    <t>RESET_RATE</t>
+  </si>
+  <si>
+    <t>security_des().value</t>
+  </si>
+  <si>
+    <t>ZH018054 Corp</t>
+  </si>
+  <si>
+    <t>BAYNGR 7 09/25/2083</t>
+  </si>
+  <si>
+    <t>BV444352 Corp</t>
+  </si>
+  <si>
+    <t>BAYNGR 5 ⅜ 03/25/2082</t>
+  </si>
+  <si>
+    <t>BN586419 Corp</t>
+  </si>
+  <si>
+    <t>TTEFP 2 ⅛ PERP</t>
+  </si>
+  <si>
+    <t>ZQ513315 Corp</t>
+  </si>
+  <si>
+    <t>BAYNGR 3 ⅛ 11/12/2079</t>
+  </si>
+  <si>
+    <t>ZO200833 Corp</t>
+  </si>
+  <si>
+    <t>TTEFP 2 PERP</t>
+  </si>
+  <si>
+    <t>ZI991241 Corp</t>
+  </si>
+  <si>
+    <t>BAYNGR 6 ⅝ 09/25/2083</t>
+  </si>
+  <si>
+    <t>EK755342 Corp</t>
+  </si>
+  <si>
+    <t>TTEFP 2 ⅝ PERP</t>
+  </si>
+  <si>
+    <t>QZ730458 Corp</t>
+  </si>
+  <si>
+    <t>TTEFP 3.369 PERP</t>
+  </si>
+  <si>
+    <t>BN586968 Corp</t>
+  </si>
+  <si>
+    <t>TTEFP 1 ⅝ PERP</t>
+  </si>
+  <si>
+    <t>BT428802 Corp</t>
+  </si>
+  <si>
+    <t>TTEFP 3 ¼ PERP</t>
+  </si>
+  <si>
+    <t>BV444257 Corp</t>
+  </si>
+  <si>
+    <t>BAYNGR 4 ½ 03/25/2082</t>
+  </si>
+  <si>
+    <t>BT431112 Corp</t>
+  </si>
+  <si>
+    <t>ZQ512606 Corp</t>
+  </si>
+  <si>
+    <t>BAYNGR 2 ⅜ 11/12/2079</t>
+  </si>
+  <si>
+    <t>BO383453 Corp</t>
+  </si>
+  <si>
+    <t>ENELIM 1 ⅞ PERP</t>
+  </si>
+  <si>
+    <t>BO383167 Corp</t>
+  </si>
+  <si>
+    <t>ENELIM 1 ⅜ PERP</t>
+  </si>
+  <si>
+    <t>ZM324570 Corp</t>
+  </si>
+  <si>
+    <t>ENELIM 6 ⅝ PERP</t>
+  </si>
+  <si>
+    <t>ZD175471 Corp</t>
+  </si>
+  <si>
+    <t>ENELIM 4 ¾ PERP</t>
+  </si>
+  <si>
+    <t>ZM324250 Corp</t>
+  </si>
+  <si>
+    <t>ENELIM 6 ⅜ PERP</t>
+  </si>
+  <si>
+    <t>AS640440 Corp</t>
+  </si>
+  <si>
+    <t>ENELIM 3 ⅜ PERP</t>
+  </si>
+  <si>
+    <t>ZS668300 Corp</t>
+  </si>
+  <si>
+    <t>ENELIM 3 ½ PERP</t>
+  </si>
+  <si>
+    <t>ZO264426 Corp</t>
+  </si>
+  <si>
+    <t>ENELIM 2 ¼ PERP</t>
+  </si>
+  <si>
+    <t>nxt_call_dt().value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -416,11 +587,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -443,10 +616,84 @@
   <volType type="realTimeData">
     <main first="bofaddin.rtdserver">
       <tp t="s">
+        <v>#N/A Requesting Data...2987910384</v>
+        <stp/>
+        <stp>BQL|16959952450720968352</stp>
+        <tr r="A1" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...3315239207</v>
+        <stp/>
+        <stp>BDP|13246031401302976869</stp>
+        <tr r="Q4" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...4045876031</v>
+        <stp/>
+        <stp>BDP|16072960715504317467</stp>
+        <tr r="T8" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...3364587050</v>
+        <stp/>
+        <stp>BDP|13513386451563173409</stp>
+        <tr r="T2" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...3518625973</v>
+        <stp/>
+        <stp>BDP|12620045661810840765</stp>
+        <tr r="T4" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...3936331402</v>
+        <stp/>
+        <stp>BDP|11692127319234153614</stp>
+        <tr r="T9" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...2977060216</v>
+        <stp/>
+        <stp>BDP|16258948000678427423</stp>
+        <tr r="Q2" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...3241551866</v>
+        <stp/>
+        <stp>BDP|13515151094479470598</stp>
+        <tr r="Q3" s="1"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A Requesting Data...3794494694</v>
+        <stp/>
+        <stp>BDP|6693911377164186675</stp>
+        <tr r="T3" s="1"/>
+      </tp>
+      <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BQL|6895208636949508967</stp>
-        <tr r="A1" s="1"/>
+        <stp>BQL|2772827279830567843</stp>
+        <tr r="A1" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...3785566059</v>
+        <stp/>
+        <stp>BDP|4686829815313545920</stp>
+        <tr r="T5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...3330400473</v>
+        <stp/>
+        <stp>BDP|8963622202360523995</stp>
+        <tr r="T6" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...3244541597</v>
+        <stp/>
+        <stp>BDP|613264357678691907</stp>
+        <tr r="T7" s="1"/>
       </tp>
     </main>
   </volType>
@@ -771,10 +1018,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B775DA10-2A92-4818-89E2-45B7F2123F30}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:T72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,10 +1030,10 @@
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
-        <f>_xll.BQL("filter(bondsuniv('active',CONSOLIDATEDUPLICATES='N'),BASEL_III_DESIGNATION=='Additional Tier 1' AND amt_outstanding(currency=EUR)&gt;=500000000 AND CRNCY=='EUR' AND BETWEEN(BB_COMPOSITE,'B','AAA'))", "security_des().value,id().value, yield(yield_type=Y" &amp; "TC).value, yield(yield_type=YTM).value, cpn().value, issue_dt().value, nxt_call_dt(), first_call_dt_issuance().value, bb_composite().value, flt_spread().value", "showids=false","cols=10;rows=51")</f>
-        <v>security_des().value</v>
+        <f>_xll.BQL("filter(bondsuniv('active',CONSOLIDATEDUPLICATES='N'),BASEL_III_DESIGNATION=='Additional Tier 1' AND amt_outstanding(currency=EUR)&gt;=500000000 AND CRNCY=='EUR' AND BETWEEN(BB_COMPOSITE,'B','AAA'))", "security_des().value,id().value, yield(yield_type=Y" &amp; "TC).value, yield(yield_type=YTM).value, cpn().value, issue_dt().value, nxt_call_dt(), first_call_dt_issuance().value, bb_composite().value, flt_spread().value, reset_index().value", "showids=false","cols=11;rows=51")</f>
+        <v>#N/A Requesting Data...</v>
       </c>
       <c r="B1" t="s">
         <v>50</v>
@@ -815,8 +1062,17 @@
       <c r="J1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -824,10 +1080,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>7.5832002173795479</v>
+        <v>7.560694242190829</v>
       </c>
       <c r="D2">
-        <v>7.6917534634162745</v>
+        <v>7.664446310406249</v>
       </c>
       <c r="E2" s="2">
         <v>8.125</v>
@@ -847,8 +1103,34 @@
       <c r="J2">
         <v>526.1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>115</v>
+      </c>
+      <c r="L2" t="str">
+        <f>VLOOKUP(K2,$P$2:$Q$7,2,FALSE)</f>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M2" t="str">
+        <f ca="1">VLOOKUP(MAX(1,ROUNDDOWN((G2-TODAY())/365,0)),$S$2:$T$9,2,FALSE)</f>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="P2" t="str" cm="1">
+        <f t="array" ref="P2:P4">_xlfn.UNIQUE(K2:K51)</f>
+        <v>EUAMDB05 Index</v>
+      </c>
+      <c r="Q2" t="str" cm="1">
+        <f t="array" ref="Q2">_xll.BDP(P2,"PX_LAST")</f>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2" t="str" cm="1">
+        <f t="array" ref="T2">_xll.BDP("EUSA"&amp;S2&amp;" Curncy","PX_LAST")</f>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -856,10 +1138,10 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>6.3715504823524816</v>
+        <v>6.3438176751607775</v>
       </c>
       <c r="D3">
-        <v>6.7176271967207866</v>
+        <v>6.7426183799073796</v>
       </c>
       <c r="E3" s="2">
         <v>7</v>
@@ -879,8 +1161,33 @@
       <c r="J3">
         <v>443.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L51" si="0">VLOOKUP(K3,$P$2:$Q$7,2,FALSE)</f>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M51" ca="1" si="1">VLOOKUP(MAX(1,ROUNDDOWN((G3-TODAY())/365,0)),$S$2:$T$9,2,FALSE)</f>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="P3" t="str">
+        <v>EUSA5 Index</v>
+      </c>
+      <c r="Q3" t="str" cm="1">
+        <f t="array" ref="Q3">_xll.BDP(P3,"PX_LAST")</f>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="S3">
+        <v>2</v>
+      </c>
+      <c r="T3" t="str" cm="1">
+        <f t="array" ref="T3">_xll.BDP("EUSA"&amp;S3&amp;" Curncy","PX_LAST")</f>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -888,10 +1195,10 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>6.7034042185481724</v>
+        <v>6.6852024174694176</v>
       </c>
       <c r="D4">
-        <v>6.7762552871168804</v>
+        <v>6.7506048789954578</v>
       </c>
       <c r="E4" s="2">
         <v>7</v>
@@ -911,8 +1218,33 @@
       <c r="J4">
         <v>435.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>115</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="P4" t="str">
+        <v>EUR003M Index</v>
+      </c>
+      <c r="Q4" t="str" cm="1">
+        <f t="array" ref="Q4">_xll.BDP(P4,"PX_LAST")</f>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="S4">
+        <v>3</v>
+      </c>
+      <c r="T4" t="str" cm="1">
+        <f t="array" ref="T4">_xll.BDP("EUSA"&amp;S4&amp;" Curncy","PX_LAST")</f>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -920,10 +1252,10 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>7.1702252337831158</v>
+        <v>7.1360505460170165</v>
       </c>
       <c r="D5">
-        <v>7.4299868671454661</v>
+        <v>7.3989757786325043</v>
       </c>
       <c r="E5" s="2">
         <v>7.875</v>
@@ -943,8 +1275,26 @@
       <c r="J5">
         <v>512.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>115</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="S5">
+        <v>4</v>
+      </c>
+      <c r="T5" t="str" cm="1">
+        <f t="array" ref="T5">_xll.BDP("EUSA"&amp;S5&amp;" Curncy","PX_LAST")</f>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -952,10 +1302,10 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>7.0953754215403748</v>
+        <v>7.021647392678716</v>
       </c>
       <c r="D6">
-        <v>7.5044171607187229</v>
+        <v>7.517900921146059</v>
       </c>
       <c r="E6" s="2">
         <v>7.875</v>
@@ -975,8 +1325,26 @@
       <c r="J6">
         <v>522.79999999999995</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="S6">
+        <v>5</v>
+      </c>
+      <c r="T6" t="str" cm="1">
+        <f t="array" ref="T6">_xll.BDP("EUSA"&amp;S6&amp;" Curncy","PX_LAST")</f>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -984,10 +1352,10 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>6.7323722682020284</v>
+        <v>6.6904159136999182</v>
       </c>
       <c r="D7">
-        <v>6.4433000931679034</v>
+        <v>6.4588654564071293</v>
       </c>
       <c r="E7" s="2">
         <v>6.875</v>
@@ -1007,8 +1375,26 @@
       <c r="J7">
         <v>426.7</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>116</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="S7">
+        <v>6</v>
+      </c>
+      <c r="T7" t="str" cm="1">
+        <f t="array" ref="T7">_xll.BDP("EUSA"&amp;S7&amp;" Curncy","PX_LAST")</f>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -1016,10 +1402,10 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>6.0267437065406115</v>
+        <v>6.0103519947008479</v>
       </c>
       <c r="D8">
-        <v>6.492599841900625</v>
+        <v>6.4672887126836072</v>
       </c>
       <c r="E8" s="2">
         <v>6.5</v>
@@ -1039,8 +1425,26 @@
       <c r="J8">
         <v>420.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>115</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="S8">
+        <v>7</v>
+      </c>
+      <c r="T8" t="str" cm="1">
+        <f t="array" ref="T8">_xll.BDP("EUSA"&amp;S8&amp;" Curncy","PX_LAST")</f>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -1048,10 +1452,10 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>6.2580718504916719</v>
+        <v>6.2152547391020194</v>
       </c>
       <c r="D9">
-        <v>6.5080806336561245</v>
+        <v>6.4755766370448136</v>
       </c>
       <c r="E9" s="2">
         <v>3.875</v>
@@ -1071,8 +1475,26 @@
       <c r="J9">
         <v>408.1</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>115</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="S9">
+        <v>8</v>
+      </c>
+      <c r="T9" t="str" cm="1">
+        <f t="array" ref="T9">_xll.BDP("EUSA"&amp;S9&amp;" Curncy","PX_LAST")</f>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -1080,10 +1502,10 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>6.7399341794175962</v>
+        <v>6.6695665135337467</v>
       </c>
       <c r="D10">
-        <v>6.9420882588433681</v>
+        <v>6.9808163188754326</v>
       </c>
       <c r="E10" s="2">
         <v>4.375</v>
@@ -1103,8 +1525,19 @@
       <c r="J10">
         <v>453.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>116</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -1112,10 +1545,10 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>7.4220627319061698</v>
+        <v>7.3940354351471802</v>
       </c>
       <c r="D11">
-        <v>6.4537482119392902</v>
+        <v>6.4227891625597398</v>
       </c>
       <c r="E11" s="2">
         <v>3.625</v>
@@ -1135,8 +1568,19 @@
       <c r="J11">
         <v>376</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>115</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>75</v>
       </c>
@@ -1144,10 +1588,10 @@
         <v>12</v>
       </c>
       <c r="C12">
-        <v>9.1861166007832615</v>
+        <v>9.0887675130423453</v>
       </c>
       <c r="D12">
-        <v>7.260648489645372</v>
+        <v>7.2191309988454107</v>
       </c>
       <c r="E12" s="2">
         <v>4.5</v>
@@ -1167,8 +1611,19 @@
       <c r="J12">
         <v>455.2</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>115</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>74</v>
       </c>
@@ -1176,10 +1631,10 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>6.0559682903293295</v>
+        <v>6.0298356956899513</v>
       </c>
       <c r="D13">
-        <v>6.7605278609129957</v>
+        <v>6.7326164172740937</v>
       </c>
       <c r="E13" s="2">
         <v>7.375</v>
@@ -1199,8 +1654,19 @@
       <c r="J13">
         <v>463.1</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>115</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -1208,10 +1674,10 @@
         <v>14</v>
       </c>
       <c r="C14">
-        <v>8.9248844292000467</v>
+        <v>8.88545797358376</v>
       </c>
       <c r="D14">
-        <v>7.4713098728554401</v>
+        <v>7.4377754741702145</v>
       </c>
       <c r="E14" s="2">
         <v>4.625</v>
@@ -1231,8 +1697,19 @@
       <c r="J14">
         <v>474.7</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>115</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>70</v>
       </c>
@@ -1240,10 +1717,10 @@
         <v>7</v>
       </c>
       <c r="C15">
-        <v>6.7874016586964609</v>
+        <v>6.7033379622371507</v>
       </c>
       <c r="D15">
-        <v>8.760767743998203</v>
+        <v>8.7208868148208882</v>
       </c>
       <c r="E15" s="2">
         <v>10</v>
@@ -1263,8 +1740,19 @@
       <c r="J15">
         <v>694</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>115</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -1272,10 +1760,10 @@
         <v>15</v>
       </c>
       <c r="C16">
-        <v>6.1104005879866872</v>
+        <v>6.1204602048021544</v>
       </c>
       <c r="D16">
-        <v>8.4549305464315765</v>
+        <v>8.4996253488492179</v>
       </c>
       <c r="E16" s="2">
         <v>6.125</v>
@@ -1295,8 +1783,19 @@
       <c r="J16">
         <v>636.29999999999995</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>116</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -1304,10 +1803,10 @@
         <v>13</v>
       </c>
       <c r="C17">
-        <v>6.2121538441883377</v>
+        <v>6.2921376088393988</v>
       </c>
       <c r="D17">
-        <v>6.5198907938070727</v>
+        <v>6.570429569306298</v>
       </c>
       <c r="E17" s="2">
         <v>3.75</v>
@@ -1327,8 +1826,19 @@
       <c r="J17">
         <v>410.2</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>116</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -1339,7 +1849,7 @@
         <v>#N/A</v>
       </c>
       <c r="D18">
-        <v>5.9439137810432277</v>
+        <v>5.9415367379439772</v>
       </c>
       <c r="E18" s="2">
         <v>5.7110000000000003</v>
@@ -1359,8 +1869,19 @@
       <c r="J18">
         <v>200</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>117</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M18" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -1368,10 +1889,10 @@
         <v>16</v>
       </c>
       <c r="C19">
-        <v>5.8125612754727491</v>
+        <v>5.7926767412884672</v>
       </c>
       <c r="D19">
-        <v>8.891173253434614</v>
+        <v>8.9275793382368054</v>
       </c>
       <c r="E19" s="2">
         <v>7.75</v>
@@ -1391,8 +1912,19 @@
       <c r="J19">
         <v>719.2</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>116</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>90</v>
       </c>
@@ -1400,10 +1932,10 @@
         <v>27</v>
       </c>
       <c r="C20">
-        <v>7.6294914700625931</v>
+        <v>7.5030315913477219</v>
       </c>
       <c r="D20">
-        <v>7.9781259377358911</v>
+        <v>7.9232971627176285</v>
       </c>
       <c r="E20" s="2">
         <v>6.75</v>
@@ -1423,8 +1955,19 @@
       <c r="J20">
         <v>569.20000000000005</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>115</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -1432,10 +1975,10 @@
         <v>18</v>
       </c>
       <c r="C21">
-        <v>5.751346496144766</v>
+        <v>5.5766279410453903</v>
       </c>
       <c r="D21">
-        <v>5.4422728702569803</v>
+        <v>5.4851881591471976</v>
       </c>
       <c r="E21" s="2">
         <v>3.5</v>
@@ -1455,8 +1998,19 @@
       <c r="J21">
         <v>300.3</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>116</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>86</v>
       </c>
@@ -1464,10 +2018,10 @@
         <v>23</v>
       </c>
       <c r="C22">
-        <v>5.8761446402893709</v>
+        <v>5.8271471810805995</v>
       </c>
       <c r="D22">
-        <v>6.1727867158655849</v>
+        <v>6.1972478923459091</v>
       </c>
       <c r="E22" s="2">
         <v>4.75</v>
@@ -1487,8 +2041,19 @@
       <c r="J22">
         <v>384.4</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>116</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>100</v>
       </c>
@@ -1496,10 +2061,10 @@
         <v>37</v>
       </c>
       <c r="C23">
-        <v>6.2658241592295685</v>
+        <v>6.218328079481938</v>
       </c>
       <c r="D23">
-        <v>6.1474012903423114</v>
+        <v>6.1844425116951971</v>
       </c>
       <c r="E23" s="2">
         <v>3.25</v>
@@ -1519,8 +2084,19 @@
       <c r="J23">
         <v>370.2</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>116</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>92</v>
       </c>
@@ -1528,10 +2104,10 @@
         <v>29</v>
       </c>
       <c r="C24">
-        <v>5.9269784484962837</v>
+        <v>5.9444431161533275</v>
       </c>
       <c r="D24">
-        <v>6.0157344324733169</v>
+        <v>6.063066496283505</v>
       </c>
       <c r="E24" s="2">
         <v>4.25</v>
@@ -1551,8 +2127,19 @@
       <c r="J24">
         <v>359.4</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>116</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -1560,10 +2147,10 @@
         <v>20</v>
       </c>
       <c r="C25">
-        <v>5.8489547314599326</v>
+        <v>5.8295022626777984</v>
       </c>
       <c r="D25">
-        <v>6.0440142940338699</v>
+        <v>6.075015308661551</v>
       </c>
       <c r="E25" s="2">
         <v>4.875</v>
@@ -1583,8 +2170,19 @@
       <c r="J25">
         <v>371.7</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>116</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>102</v>
       </c>
@@ -1592,10 +2190,10 @@
         <v>39</v>
       </c>
       <c r="C26">
-        <v>5.4609964318950874</v>
+        <v>5.2942732845530127</v>
       </c>
       <c r="D26">
-        <v>8.700063060367917</v>
+        <v>8.7342771816142992</v>
       </c>
       <c r="E26" s="2">
         <v>6.25</v>
@@ -1615,8 +2213,19 @@
       <c r="J26">
         <v>662.9</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>116</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -1624,10 +2233,10 @@
         <v>19</v>
       </c>
       <c r="C27">
-        <v>6.2103445156890018</v>
+        <v>6.1510142793470504</v>
       </c>
       <c r="D27">
-        <v>7.8892287396884591</v>
+        <v>7.8532127255009287</v>
       </c>
       <c r="E27" s="2">
         <v>9.125</v>
@@ -1647,8 +2256,19 @@
       <c r="J27">
         <v>626.20000000000005</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>115</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>96</v>
       </c>
@@ -1656,10 +2276,10 @@
         <v>33</v>
       </c>
       <c r="C28">
-        <v>8.314577733911122</v>
+        <v>8.285547735750546</v>
       </c>
       <c r="D28">
-        <v>6.0516801632838986</v>
+        <v>6.085565229684117</v>
       </c>
       <c r="E28" s="2">
         <v>3</v>
@@ -1679,8 +2299,19 @@
       <c r="J28">
         <v>312.10000000000002</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>116</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>89</v>
       </c>
@@ -1688,10 +2319,10 @@
         <v>26</v>
       </c>
       <c r="C29">
-        <v>6.5423863043854489</v>
+        <v>6.4852748021976225</v>
       </c>
       <c r="D29">
-        <v>6.7729989314798527</v>
+        <v>6.7355185726420892</v>
       </c>
       <c r="E29" s="2">
         <v>7.125</v>
@@ -1711,8 +2342,19 @@
       <c r="J29">
         <v>438.7</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" t="s">
+        <v>115</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>103</v>
       </c>
@@ -1720,10 +2362,10 @@
         <v>40</v>
       </c>
       <c r="C30">
-        <v>9.61375528766232</v>
+        <v>9.6033089833610248</v>
       </c>
       <c r="D30">
-        <v>5.5085067793659537</v>
+        <v>5.5547794614805142</v>
       </c>
       <c r="E30" s="2">
         <v>3.625</v>
@@ -1743,328 +2385,449 @@
       <c r="J30">
         <v>293.8</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>116</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C31">
-        <v>5.6958239129765582</v>
+        <v>6.2456027235166491</v>
       </c>
       <c r="D31">
-        <v>6.6290519875301719</v>
+        <v>7.5671012573319532</v>
       </c>
       <c r="E31" s="2">
-        <v>7.25</v>
+        <v>6.375</v>
       </c>
       <c r="F31" s="1">
-        <v>44936</v>
+        <v>44650</v>
       </c>
       <c r="G31" s="3">
-        <v>47019</v>
+        <v>46842</v>
       </c>
       <c r="H31" s="3">
-        <v>47019</v>
+        <v>46842</v>
       </c>
       <c r="I31" t="s">
+        <v>60</v>
+      </c>
+      <c r="J31">
+        <v>555.5</v>
+      </c>
+      <c r="K31" t="s">
+        <v>116</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M31" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32">
+        <v>5.8681425751943612</v>
+      </c>
+      <c r="D32">
+        <v>6.7448939925031324</v>
+      </c>
+      <c r="E32" s="2">
+        <v>6.875</v>
+      </c>
+      <c r="F32" s="1">
+        <v>44810</v>
+      </c>
+      <c r="G32" s="3">
+        <v>47458</v>
+      </c>
+      <c r="H32" s="3">
+        <v>47458</v>
+      </c>
+      <c r="I32" t="s">
         <v>61</v>
       </c>
-      <c r="J31">
-        <v>444.1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>85</v>
-      </c>
-      <c r="B32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32">
-        <v>6.2853555336843474</v>
-      </c>
-      <c r="D32">
-        <v>7.5402257737460072</v>
-      </c>
-      <c r="E32" s="2">
-        <v>6.375</v>
-      </c>
-      <c r="F32" s="1">
-        <v>44650</v>
-      </c>
-      <c r="G32" s="3">
-        <v>46842</v>
-      </c>
-      <c r="H32" s="3">
-        <v>46842</v>
-      </c>
-      <c r="I32" t="s">
+      <c r="J32">
+        <v>464.5</v>
+      </c>
+      <c r="K32" t="s">
+        <v>116</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33">
+        <v>5.4074667289157725</v>
+      </c>
+      <c r="D33">
+        <v>7.5918451791658494</v>
+      </c>
+      <c r="E33" s="2">
+        <v>4.9470000000000001</v>
+      </c>
+      <c r="F33" s="1">
+        <v>41730</v>
+      </c>
+      <c r="G33" s="3">
+        <v>45835</v>
+      </c>
+      <c r="H33" s="3">
+        <v>44009</v>
+      </c>
+      <c r="I33" t="s">
+        <v>59</v>
+      </c>
+      <c r="J33">
+        <v>529</v>
+      </c>
+      <c r="K33" t="s">
+        <v>115</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34">
+        <v>6.6016504674812335</v>
+      </c>
+      <c r="D34">
+        <v>6.7080702876085141</v>
+      </c>
+      <c r="E34" s="2">
+        <v>4.125</v>
+      </c>
+      <c r="F34" s="1">
+        <v>43888</v>
+      </c>
+      <c r="G34" s="3">
+        <v>47541</v>
+      </c>
+      <c r="H34" s="3">
+        <v>47541</v>
+      </c>
+      <c r="I34" t="s">
         <v>60</v>
       </c>
-      <c r="J32">
-        <v>555.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>91</v>
-      </c>
-      <c r="B33" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33">
-        <v>5.9225788961811743</v>
-      </c>
-      <c r="D33">
-        <v>6.727216114586466</v>
-      </c>
-      <c r="E33" s="2">
-        <v>6.875</v>
-      </c>
-      <c r="F33" s="1">
-        <v>44810</v>
-      </c>
-      <c r="G33" s="3">
-        <v>47458</v>
-      </c>
-      <c r="H33" s="3">
-        <v>47458</v>
-      </c>
-      <c r="I33" t="s">
-        <v>61</v>
-      </c>
-      <c r="J33">
-        <v>464.5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>101</v>
-      </c>
-      <c r="B34" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34">
-        <v>5.5801365355179708</v>
-      </c>
-      <c r="D34">
-        <v>7.629255162001809</v>
-      </c>
-      <c r="E34" s="2">
-        <v>4.9470000000000001</v>
-      </c>
-      <c r="F34" s="1">
-        <v>41730</v>
-      </c>
-      <c r="G34" s="3">
-        <v>45835</v>
-      </c>
-      <c r="H34" s="3">
-        <v>44009</v>
-      </c>
-      <c r="I34" t="s">
-        <v>59</v>
-      </c>
       <c r="J34">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+        <v>427.4</v>
+      </c>
+      <c r="K34" t="s">
+        <v>116</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C35">
-        <v>6.640010480829619</v>
+        <v>7.7400654975216403</v>
       </c>
       <c r="D35">
-        <v>6.6841022153372709</v>
+        <v>6.9481966869552982</v>
       </c>
       <c r="E35" s="2">
-        <v>4.125</v>
+        <v>4.25</v>
       </c>
       <c r="F35" s="1">
-        <v>43888</v>
+        <v>44369</v>
       </c>
       <c r="G35" s="3">
-        <v>47541</v>
+        <v>46669</v>
       </c>
       <c r="H35" s="3">
-        <v>47541</v>
+        <v>46669</v>
       </c>
       <c r="I35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J35">
-        <v>427.4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+        <v>438.7</v>
+      </c>
+      <c r="K35" t="s">
+        <v>116</v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M35" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C36">
-        <v>7.8034451127927422</v>
+        <v>5.6316641218077326</v>
       </c>
       <c r="D36">
-        <v>6.9202873647943823</v>
+        <v>8.5670981144308005</v>
       </c>
       <c r="E36" s="2">
-        <v>4.25</v>
+        <v>6</v>
       </c>
       <c r="F36" s="1">
-        <v>44369</v>
+        <v>44027</v>
       </c>
       <c r="G36" s="3">
-        <v>46669</v>
+        <v>46037</v>
       </c>
       <c r="H36" s="3">
-        <v>46669</v>
+        <v>46037</v>
       </c>
       <c r="I36" t="s">
         <v>58</v>
       </c>
       <c r="J36">
-        <v>438.7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>645.6</v>
+      </c>
+      <c r="K36" t="s">
+        <v>116</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M36" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C37">
-        <v>5.6226525628767812</v>
+        <v>5.7919156551840532</v>
       </c>
       <c r="D37">
-        <v>8.5212635647403729</v>
+        <v>6.572950166771288</v>
       </c>
       <c r="E37" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F37" s="1">
-        <v>44027</v>
+        <v>44118</v>
       </c>
       <c r="G37" s="3">
-        <v>46037</v>
+        <v>46744</v>
       </c>
       <c r="H37" s="3">
-        <v>46037</v>
+        <v>46744</v>
       </c>
       <c r="I37" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="J37">
-        <v>645.6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+        <v>437</v>
+      </c>
+      <c r="K37" t="s">
+        <v>116</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M37" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B38" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C38">
-        <v>5.8275567463795017</v>
+        <v>5.882733503115138</v>
       </c>
       <c r="D38">
-        <v>6.5416174319589668</v>
+        <v>9.1954638506287552</v>
       </c>
       <c r="E38" s="2">
-        <v>4</v>
+        <v>7.5</v>
       </c>
       <c r="F38" s="1">
-        <v>44118</v>
+        <v>43543</v>
       </c>
       <c r="G38" s="3">
-        <v>46744</v>
+        <v>46176</v>
       </c>
       <c r="H38" s="3">
-        <v>46744</v>
+        <v>46176</v>
       </c>
       <c r="I38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J38">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <v>733.4</v>
+      </c>
+      <c r="K38" t="s">
+        <v>115</v>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M38" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C39">
-        <v>5.9019577226469613</v>
+        <v>4.9851638572888719</v>
       </c>
       <c r="D39">
-        <v>9.2200530434563923</v>
+        <v>9.899753804893848</v>
       </c>
       <c r="E39" s="2">
         <v>7.5</v>
       </c>
       <c r="F39" s="1">
-        <v>43543</v>
+        <v>43970</v>
       </c>
       <c r="G39" s="3">
-        <v>46176</v>
+        <v>45796</v>
       </c>
       <c r="H39" s="3">
-        <v>46176</v>
+        <v>45796</v>
       </c>
       <c r="I39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J39">
-        <v>733.4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+        <v>792.4</v>
+      </c>
+      <c r="K39" t="s">
+        <v>116</v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M39" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B40" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C40">
-        <v>5.1581935891721704</v>
+        <v>5.6789420855291093</v>
       </c>
       <c r="D40">
-        <v>9.8647473274641317</v>
+        <v>6.6037642970921073</v>
       </c>
       <c r="E40" s="2">
-        <v>7.5</v>
+        <v>7.25</v>
       </c>
       <c r="F40" s="1">
-        <v>43970</v>
+        <v>44936</v>
       </c>
       <c r="G40" s="3">
-        <v>45796</v>
+        <v>47019</v>
       </c>
       <c r="H40" s="3">
-        <v>45796</v>
+        <v>47019</v>
       </c>
       <c r="I40" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="J40">
-        <v>792.4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+        <v>444.1</v>
+      </c>
+      <c r="K40" t="s">
+        <v>115</v>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M40" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -2072,10 +2835,10 @@
         <v>35</v>
       </c>
       <c r="C41">
-        <v>6.6533377198411729</v>
+        <v>6.6000692038506799</v>
       </c>
       <c r="D41">
-        <v>6.6540196569725065</v>
+        <v>6.6828229018864969</v>
       </c>
       <c r="E41" s="2">
         <v>4.125</v>
@@ -2095,8 +2858,19 @@
       <c r="J41">
         <v>431.1</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41" t="s">
+        <v>116</v>
+      </c>
+      <c r="L41" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M41" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>105</v>
       </c>
@@ -2104,10 +2878,10 @@
         <v>42</v>
       </c>
       <c r="C42">
-        <v>6.0213344357026921</v>
+        <v>5.9793114104927785</v>
       </c>
       <c r="D42">
-        <v>7.749987997511437</v>
+        <v>7.7775653568204239</v>
       </c>
       <c r="E42" s="2">
         <v>5.5</v>
@@ -2127,8 +2901,19 @@
       <c r="J42">
         <v>584.79999999999995</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K42" t="s">
+        <v>116</v>
+      </c>
+      <c r="L42" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>95</v>
       </c>
@@ -2136,10 +2921,10 @@
         <v>32</v>
       </c>
       <c r="C43">
-        <v>6.0189614939262688</v>
+        <v>5.9656419109614651</v>
       </c>
       <c r="D43">
-        <v>7.5148427792422012</v>
+        <v>7.4817775851353039</v>
       </c>
       <c r="E43" s="2">
         <v>8.375</v>
@@ -2159,8 +2944,19 @@
       <c r="J43">
         <v>554.4</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K43" t="s">
+        <v>115</v>
+      </c>
+      <c r="L43" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M43" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>107</v>
       </c>
@@ -2168,10 +2964,10 @@
         <v>44</v>
       </c>
       <c r="C44">
-        <v>5.7829201926015124</v>
+        <v>5.7354478682762124</v>
       </c>
       <c r="D44">
-        <v>7.0101085812026813</v>
+        <v>6.9779900808980715</v>
       </c>
       <c r="E44" s="2">
         <v>8</v>
@@ -2191,8 +2987,19 @@
       <c r="J44">
         <v>492.8</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K44" t="s">
+        <v>115</v>
+      </c>
+      <c r="L44" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M44" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>106</v>
       </c>
@@ -2200,10 +3007,10 @@
         <v>43</v>
       </c>
       <c r="C45">
-        <v>6.0292800821957693</v>
+        <v>6.0074112556188135</v>
       </c>
       <c r="D45">
-        <v>7.5125508212403558</v>
+        <v>7.5320114326956453</v>
       </c>
       <c r="E45" s="2">
         <v>5.875</v>
@@ -2223,8 +3030,19 @@
       <c r="J45">
         <v>608.6</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K45" t="s">
+        <v>116</v>
+      </c>
+      <c r="L45" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M45" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>110</v>
       </c>
@@ -2232,10 +3050,10 @@
         <v>47</v>
       </c>
       <c r="C46">
-        <v>6.5054941027566029</v>
+        <v>6.4509641968334597</v>
       </c>
       <c r="D46">
-        <v>5.7599827355068154</v>
+        <v>5.7891707108967516</v>
       </c>
       <c r="E46" s="2">
         <v>3.1</v>
@@ -2255,8 +3073,19 @@
       <c r="J46">
         <v>323.39999999999998</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K46" t="s">
+        <v>116</v>
+      </c>
+      <c r="L46" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M46" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>109</v>
       </c>
@@ -2264,10 +3093,10 @@
         <v>46</v>
       </c>
       <c r="C47">
-        <v>5.6686322290526769</v>
+        <v>5.6146683768047652</v>
       </c>
       <c r="D47">
-        <v>6.7876323312128752</v>
+        <v>6.8174866893200523</v>
       </c>
       <c r="E47" s="2">
         <v>4.375</v>
@@ -2287,8 +3116,19 @@
       <c r="J47">
         <v>467.9</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K47" t="s">
+        <v>116</v>
+      </c>
+      <c r="L47" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M47" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>104</v>
       </c>
@@ -2296,10 +3136,10 @@
         <v>41</v>
       </c>
       <c r="C48">
-        <v>5.7748137913994881</v>
+        <v>5.7910767326171984</v>
       </c>
       <c r="D48">
-        <v>6.464732836322038</v>
+        <v>6.5115262731863028</v>
       </c>
       <c r="E48" s="2">
         <v>4.625</v>
@@ -2319,8 +3159,19 @@
       <c r="J48">
         <v>409.8</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K48" t="s">
+        <v>116</v>
+      </c>
+      <c r="L48" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M48" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>108</v>
       </c>
@@ -2328,10 +3179,10 @@
         <v>45</v>
       </c>
       <c r="C49">
-        <v>6.442180575322344</v>
+        <v>6.4091863467360008</v>
       </c>
       <c r="D49">
-        <v>8.1908647387473206</v>
+        <v>8.2107253572739669</v>
       </c>
       <c r="E49" s="2">
         <v>6.5</v>
@@ -2351,8 +3202,19 @@
       <c r="J49">
         <v>674.3</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K49" t="s">
+        <v>116</v>
+      </c>
+      <c r="L49" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M49" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>112</v>
       </c>
@@ -2360,10 +3222,10 @@
         <v>49</v>
       </c>
       <c r="C50">
-        <v>7.2889888910471861</v>
+        <v>7.3114125003764538</v>
       </c>
       <c r="D50">
-        <v>6.4924057883723698</v>
+        <v>6.4670842266044648</v>
       </c>
       <c r="E50" s="2">
         <v>3.875</v>
@@ -2383,8 +3245,19 @@
       <c r="J50">
         <v>401</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K50" t="s">
+        <v>115</v>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M50" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>111</v>
       </c>
@@ -2392,10 +3265,10 @@
         <v>48</v>
       </c>
       <c r="C51">
-        <v>5.4329144589389262</v>
+        <v>5.408561488525871</v>
       </c>
       <c r="D51">
-        <v>6.7519762825107472</v>
+        <v>6.7920097428170632</v>
       </c>
       <c r="E51" s="2">
         <v>4.125</v>
@@ -2415,80 +3288,91 @@
       <c r="J51">
         <v>456.8</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K51" t="s">
+        <v>116</v>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="0"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+      <c r="M51" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>#N/A Requesting Data...</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E52" s="2"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E53" s="2"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E54" s="2"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E55" s="2"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E56" s="2"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E57" s="2"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E58" s="2"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E59" s="2"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E60" s="2"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E61" s="2"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E62" s="2"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E63" s="2"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E64" s="2"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -2546,4 +3430,527 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53A5D76-2B01-45A1-9CE0-F9CB1DA6184D}">
+  <dimension ref="A1:L171"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="str">
+        <f>_xll.BQL("filter(bondsuniv(ACTIVE),is_subordinated()== 'Y' and ticker() in ['TTEFP','ENELIM', 'BAYNGR'])", "security_des().value, yield(yield_type=YTC).value, nxt_call_dt().value","cols=4;rows=22")</f>
+        <v>ID</v>
+      </c>
+      <c r="B1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="5">
+        <v>4.8491078022117673</v>
+      </c>
+      <c r="D2" s="3">
+        <v>47642</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="5">
+        <v>5.6713939911744964</v>
+      </c>
+      <c r="D3" s="3">
+        <v>48116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="5">
+        <v>5.5346718911116826</v>
+      </c>
+      <c r="D4" s="3">
+        <v>47659</v>
+      </c>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4.7092515876915231</v>
+      </c>
+      <c r="D5" s="3">
+        <v>46546</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="5">
+        <v>4.7514726241710932</v>
+      </c>
+      <c r="D6" s="3">
+        <v>47954</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="5">
+        <v>4.516646160067264</v>
+      </c>
+      <c r="D7" s="3">
+        <v>48420</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="5">
+        <v>4.5281383000139437</v>
+      </c>
+      <c r="D8" s="3">
+        <v>47177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="5">
+        <v>5.1690234020453314</v>
+      </c>
+      <c r="D9" s="3">
+        <v>46611</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" s="5">
+        <v>4.2259444072794432</v>
+      </c>
+      <c r="D10" s="3">
+        <v>47638</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" s="5">
+        <v>5.3641862925814783</v>
+      </c>
+      <c r="D11" s="3">
+        <v>47021</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" s="5">
+        <v>4.2623031227404518</v>
+      </c>
+      <c r="D12" s="3">
+        <v>45714</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" s="5">
+        <v>4.0635770132357001</v>
+      </c>
+      <c r="D13" s="3">
+        <v>46301</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="5">
+        <v>4.2006221659215077</v>
+      </c>
+      <c r="D14" s="3">
+        <v>46685</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C15" s="5">
+        <v>4.6430317557768923</v>
+      </c>
+      <c r="D15" s="3">
+        <v>49873</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C16" s="5">
+        <v>4.393882290105358</v>
+      </c>
+      <c r="D16" s="3">
+        <v>46859</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>156</v>
+      </c>
+      <c r="B17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="5">
+        <v>4.4390027655610815</v>
+      </c>
+      <c r="D17" s="3">
+        <v>46258</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" s="5">
+        <v>4.9810498050912715</v>
+      </c>
+      <c r="D18" s="3">
+        <v>46563</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B19" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="5">
+        <v>4.1839019819418874</v>
+      </c>
+      <c r="D19" s="3">
+        <v>46404</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B20" t="s">
+        <v>159</v>
+      </c>
+      <c r="C20" s="5">
+        <v>4.8246430468819979</v>
+      </c>
+      <c r="D20" s="3">
+        <v>45712</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>160</v>
+      </c>
+      <c r="B21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C21" s="5">
+        <v>4.4687232457982908</v>
+      </c>
+      <c r="D21" s="3">
+        <v>46366</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>144</v>
+      </c>
+      <c r="B22" t="s">
+        <v>145</v>
+      </c>
+      <c r="C22" s="5">
+        <v>4.9733515891549489</v>
+      </c>
+      <c r="D22" s="3">
+        <v>45700</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="3"/>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C87" s="3"/>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C88" s="3"/>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C89" s="3"/>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C90" s="3"/>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C91" s="3"/>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C92" s="3"/>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C93" s="3"/>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C94" s="3"/>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C95" s="3"/>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C96" s="3"/>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C97" s="3"/>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C98" s="3"/>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C99" s="3"/>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C100" s="3"/>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C101" s="3"/>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C102" s="3"/>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C103" s="3"/>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C104" s="3"/>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C105" s="3"/>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C106" s="3"/>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C107" s="3"/>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C108" s="3"/>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C109" s="3"/>
+    </row>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C110" s="3"/>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C112" s="3"/>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C113" s="3"/>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C114" s="3"/>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C115" s="3"/>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C117" s="3"/>
+    </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C119" s="3"/>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C120" s="3"/>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C122" s="3"/>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C123" s="3"/>
+    </row>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C124" s="3"/>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C126" s="3"/>
+    </row>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C128" s="3"/>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C129" s="3"/>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C130" s="3"/>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C131" s="3"/>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C132" s="3"/>
+    </row>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C134" s="3"/>
+    </row>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C137" s="3"/>
+    </row>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C141" s="3"/>
+    </row>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C142" s="3"/>
+    </row>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C143" s="3"/>
+    </row>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C144" s="3"/>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C145" s="3"/>
+    </row>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C146" s="3"/>
+    </row>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C147" s="3"/>
+    </row>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C148" s="3"/>
+    </row>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C149" s="3"/>
+    </row>
+    <row r="150" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C150" s="3"/>
+    </row>
+    <row r="151" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C151" s="3"/>
+    </row>
+    <row r="153" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C153" s="3"/>
+    </row>
+    <row r="154" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C154" s="3"/>
+    </row>
+    <row r="157" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C157" s="3"/>
+    </row>
+    <row r="158" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C158" s="3"/>
+    </row>
+    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C165" s="3"/>
+    </row>
+    <row r="168" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C168" s="3"/>
+    </row>
+    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C170" s="3"/>
+    </row>
+    <row r="171" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C171" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>